<commit_message>
Change cahier des charges techniques
</commit_message>
<xml_diff>
--- a/Cahier des charges technique.xlsx
+++ b/Cahier des charges technique.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nobil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6620137-F7E1-49FE-8FA0-6B0E3150866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D604C6-6CA1-4B87-955D-8DAB76E0C1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAGE-1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
   <si>
     <t>Nom du groupe :</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Sout. Finale</t>
   </si>
   <si>
-    <t>Team Blueberry</t>
-  </si>
-  <si>
     <t>Nobilet</t>
   </si>
   <si>
@@ -286,9 +283,6 @@
     <t>Clement</t>
   </si>
   <si>
-    <t>Raylan</t>
-  </si>
-  <si>
     <t>Charbonnier</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
     <t>clement.charbonnier@epita.fr</t>
   </si>
   <si>
-    <t>Jeu : Multi, à max 5. Chaque joueur commence sans rien, explore la map commune puis au fur et à mesure du jeu se développe pour battre un boss final.</t>
-  </si>
-  <si>
     <t>Level design (faire en sorte que les joueurs explorent = seul mais se regroupe = multi)</t>
   </si>
   <si>
@@ -325,9 +316,6 @@
     <t>Com (site web, insta ?, steam, regles, credits etc…)</t>
   </si>
   <si>
-    <t>mob</t>
-  </si>
-  <si>
     <t>graphismes</t>
   </si>
   <si>
@@ -343,14 +331,59 @@
     <t>Version de base</t>
   </si>
   <si>
-    <t>Mécaniques / physique</t>
+    <t>Team Nika</t>
+  </si>
+  <si>
+    <t>Physique</t>
+  </si>
+  <si>
+    <t>Mécaniques / personnages</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Tout le monde</t>
+  </si>
+  <si>
+    <t>Level design</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Graphismes</t>
+  </si>
+  <si>
+    <t>Mecaniques de bases</t>
+  </si>
+  <si>
+    <t>Mécaniques +</t>
+  </si>
+  <si>
+    <t>Règles</t>
+  </si>
+  <si>
+    <t>Menu or jeu</t>
+  </si>
+  <si>
+    <t>Menu en jeu</t>
+  </si>
+  <si>
+    <t>Still alone</t>
+  </si>
+  <si>
+    <t>Groupe : 5 étudiants à l'EPITA, qui vont partir à la découverte du nouveau monde comme Luffy au chapeau de paille. Notre premier ennemi sera Pythonland.               Jeu : Coop multijoueur (5max) d'exploration. Vous vous retrouvez dans les souterrains du royaume (2d one shot) pour tuer le boss et arriver à s'echapper.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -388,6 +421,12 @@
       <color theme="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -579,7 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -618,38 +657,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -674,78 +731,82 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1151,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1164,39 +1225,39 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
@@ -1205,87 +1266,87 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="22"/>
+      <c r="C7" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="47"/>
       <c r="E7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="22"/>
+      <c r="C8" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="47"/>
       <c r="E8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="22"/>
+      <c r="C9" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="47"/>
       <c r="E9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="22"/>
+        <v>84</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="47"/>
       <c r="E10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
@@ -1296,144 +1357,144 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="49"/>
+      <c r="A13" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="50"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="52"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="52"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="50"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="50"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
     </row>
     <row r="26" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -1447,13 +1508,13 @@
       <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -1461,16 +1522,16 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="6" t="s">
@@ -1478,16 +1539,16 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="6" t="s">
@@ -1498,41 +1559,41 @@
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
     </row>
     <row r="33" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="45"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="15" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="15" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1540,7 +1601,7 @@
       <c r="A36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -1549,7 +1610,7 @@
       <c r="D36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="27"/>
+      <c r="E36" s="33"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
@@ -1558,28 +1619,28 @@
       <c r="B37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="28"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
     </row>
     <row r="39" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="15" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -1603,55 +1664,55 @@
       <c r="D40" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="25"/>
+      <c r="E40" s="30"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="44" t="s">
+      <c r="C41" s="15" t="s">
         <v>54</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="25"/>
+      <c r="E41" s="30"/>
     </row>
     <row r="42" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="25"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
@@ -1660,37 +1721,37 @@
       <c r="B45" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E45" s="25"/>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
     </row>
     <row r="48" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="15" t="s">
         <v>53</v>
       </c>
       <c r="C48" s="8" t="s">
@@ -1702,28 +1763,40 @@
       <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
     </row>
     <row r="50" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
     </row>
     <row r="51" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E25"/>
@@ -1740,18 +1813,6 @@
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{C7984976-5428-427E-8AF2-BD8E6FE6E81B}"/>
@@ -1761,7 +1822,7 @@
     <hyperlink ref="C10" r:id="rId5" xr:uid="{BCCA03EC-1A5A-44A1-BFE1-25CAD4902A02}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1770,7 +1831,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1779,14 +1840,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1805,134 +1866,146 @@
         <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="108" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="57"/>
+      <c r="C4" s="61" t="s">
+        <v>104</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="56"/>
+      <c r="E4" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="58"/>
     </row>
     <row r="5" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="58"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="58"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>99</v>
+      <c r="A7" s="59" t="s">
+        <v>108</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="57"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="27" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>105</v>
+      <c r="A9" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="56"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="56"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
+        <v>97</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="56"/>
+        <v>98</v>
+      </c>
+      <c r="B11" s="17"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="58"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="56"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="27" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="56"/>
+        <v>100</v>
+      </c>
+      <c r="B13" s="16"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="56"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="17"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
@@ -1959,29 +2032,29 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
     </row>
     <row r="20" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="11" t="s">
         <v>71</v>
       </c>
@@ -1993,137 +2066,221 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="A21" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="66">
+        <v>1</v>
+      </c>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="A22" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="66">
+        <v>1</v>
+      </c>
+      <c r="F22" s="66"/>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="A23" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="66">
+        <v>0.75</v>
+      </c>
+      <c r="F23" s="66">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="A24" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="66">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="66">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="A25" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="66">
+        <v>0.4</v>
+      </c>
+      <c r="E25" s="66">
+        <v>0.75</v>
+      </c>
+      <c r="F25" s="66">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="A26" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="66">
+        <v>0</v>
+      </c>
+      <c r="E26" s="66">
+        <v>0.3</v>
+      </c>
+      <c r="F26" s="66">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="A27" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="66">
+        <v>1</v>
+      </c>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
     </row>
     <row r="28" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="A28" s="65" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="66">
+        <v>0</v>
+      </c>
+      <c r="E28" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="66">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="A29" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="E29" s="66">
+        <v>1</v>
+      </c>
+      <c r="F29" s="66"/>
     </row>
     <row r="30" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="A30" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="E30" s="66">
+        <v>1</v>
+      </c>
+      <c r="F30" s="66"/>
     </row>
     <row r="31" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="A31" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="66">
+        <v>0.1</v>
+      </c>
+      <c r="E31" s="66">
+        <v>0.6</v>
+      </c>
+      <c r="F31" s="66">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="A32" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="66">
+        <v>0.3</v>
+      </c>
+      <c r="E32" s="66">
+        <v>1</v>
+      </c>
+      <c r="F32" s="66"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
+      <c r="A33" s="56"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
+      <c r="A35" s="56"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="40"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:F19"/>
@@ -2140,12 +2297,8 @@
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>